<commit_message>
fix excel y vns
</commit_message>
<xml_diff>
--- a/Algebra y Estadistica/7- clase 5-6-24/condicionales buscarv if.xlsx
+++ b/Algebra y Estadistica/7- clase 5-6-24/condicionales buscarv if.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emi\Documents\ITU DESARROLLO\Segundo Semestre\Algebra y Estadistica\7- clase 5-6-24\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Desarrollo De Software 2023 Junin\Segundo Semestre\Algebra y Estadistica\7- clase 5-6-24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F079564C-F475-4E0F-BC85-0E9590651835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF2C40C2-981D-43CB-9AE8-2BFF6D3D49AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{0C57C015-FE4E-4771-B8BE-6F1CA9C18B52}"/>
   </bookViews>
@@ -125,8 +125,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -190,10 +190,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,7 +511,7 @@
   <dimension ref="A1:T19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,7 +680,7 @@
       </c>
       <c r="M3" s="11">
         <f ca="1">YEARFRAC(M2,NOW())</f>
-        <v>25.322222222222223</v>
+        <v>25.327777777777779</v>
       </c>
       <c r="N3" t="s">
         <v>14</v>
@@ -758,7 +758,7 @@
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D5" s="1">
         <f ca="1">TODAY()</f>
-        <v>45448</v>
+        <v>45450</v>
       </c>
       <c r="F5" s="7">
         <f>MONTH(F3)</f>
@@ -778,7 +778,7 @@
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D6" s="9">
         <f ca="1">NOW()</f>
-        <v>45448.501031018517</v>
+        <v>45450.923976388891</v>
       </c>
       <c r="F6" s="7">
         <f>DAY(F3)</f>
@@ -807,7 +807,7 @@
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D8" s="10">
         <f ca="1">D6-D7</f>
-        <v>9248.5010310185171</v>
+        <v>9250.9239763888909</v>
       </c>
       <c r="F8" s="7">
         <f>WEEKDAY(F3)</f>
@@ -871,49 +871,106 @@
       <c r="A12">
         <v>101</v>
       </c>
+      <c r="B12" t="str">
+        <f>_xlfn.XLOOKUP(A12,A17:A19,B17:B19,"ERROR")</f>
+        <v>Tita</v>
+      </c>
       <c r="C12">
+        <f>_xlfn.XLOOKUP(A12,A17:A19,C17:C19,"ERROR")</f>
         <v>150</v>
+      </c>
+      <c r="D12" s="2">
+        <v>3</v>
       </c>
       <c r="E12" s="2">
         <f>D12*C12</f>
-        <v>0</v>
+        <v>450</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>102</v>
       </c>
+      <c r="B13" t="str">
+        <f>_xlfn.XLOOKUP(A13,A18:A20,B18:B20,"ERROR")</f>
+        <v>Rodhesia</v>
+      </c>
+      <c r="C13">
+        <f t="shared" ref="C13:C15" si="5">_xlfn.XLOOKUP(A13,A18:A20,C18:C20,"ERROR")</f>
+        <v>200</v>
+      </c>
+      <c r="D13" s="2">
+        <v>4</v>
+      </c>
+      <c r="E13" s="2">
+        <f t="shared" ref="E13:E14" si="6">D13*C13</f>
+        <v>800</v>
+      </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>201</v>
       </c>
+      <c r="B14" t="str">
+        <f>_xlfn.XLOOKUP(A14,A19:A21,B19:B21,"ERROR")</f>
+        <v>Guaymallen</v>
+      </c>
       <c r="C14">
+        <f t="shared" si="5"/>
         <v>1200</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D14" s="2">
+        <v>12</v>
+      </c>
+      <c r="E14" s="2">
+        <f t="shared" si="6"/>
+        <v>14400</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>203</v>
+      </c>
+      <c r="B15" t="str">
+        <f>_xlfn.XLOOKUP(A15,A20:A22,B20:B22,"ERROR")</f>
+        <v>ERROR</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="5"/>
+        <v>ERROR</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>101</v>
       </c>
       <c r="B17" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>102</v>
       </c>
       <c r="B18" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>103</v>
+        <v>201</v>
       </c>
       <c r="B19" t="s">
         <v>27</v>
+      </c>
+      <c r="C19">
+        <v>1200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>